<commit_message>
added csv file support
</commit_message>
<xml_diff>
--- a/src/main/resources/sheet.xlsx
+++ b/src/main/resources/sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JavaProjects\RefinementTask\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EE6E99-FA59-4725-A492-82434E7C83FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E4D6D9-9DB9-4BC5-9D09-D89041F4071B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{EAC9966B-B3DB-430F-B1A7-38919990EEB5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Client Name</t>
   </si>
@@ -65,19 +65,40 @@
     <t>f</t>
   </si>
   <si>
-    <t>s1324</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>asf</t>
-  </si>
-  <si>
-    <t>sff</t>
-  </si>
-  <si>
-    <t>new_data</t>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>Z1</t>
   </si>
 </sst>
 </file>
@@ -114,8 +135,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -430,15 +452,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F698C7A-E726-4100-8E2B-0F748B41D44D}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,7 +474,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -460,13 +482,17 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <f>B2+E2*E2</f>
+        <v>2</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -474,13 +500,17 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D13" si="0">B3+E3*E3</f>
+        <v>6</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -488,13 +518,17 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -502,27 +536,35 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6" si="1">B6+E6*E6</f>
+        <v>34</v>
+      </c>
+      <c r="E6" s="1">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -530,55 +572,206 @@
         <v>6</v>
       </c>
       <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="E7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="E8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="E9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="D7" t="s">
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="E10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="E11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8">
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>132</v>
+      </c>
+      <c r="E12" s="1">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>156</v>
+      </c>
+      <c r="E13" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>6</v>
-      </c>
-      <c r="C9">
+      <c r="D14">
+        <f t="shared" ref="D14:D16" si="2">B14+E14*E14</f>
+        <v>110</v>
+      </c>
+      <c r="E14" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>132</v>
+      </c>
+      <c r="E15" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
         <v>12</v>
       </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>156</v>
+      </c>
+      <c r="E16" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>